<commit_message>
将测试Excel中 TemplateGo 改为 XlsxTemplate
</commit_message>
<xml_diff>
--- a/XlsxTemplateTests/data/go.xlsx
+++ b/XlsxTemplateTests/data/go.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanglb\work\template-go\TemplateGOTests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanglb\work\xlsx-template\XlsxTemplateTests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7C432E-B93E-47E1-93BA-DC8981B478A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80141EB-5236-44B4-9EE2-EC025BC85F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="660" windowWidth="16335" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="997" windowWidth="20565" windowHeight="13801" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -39,10 +39,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
-    <t>TemplateGO 测试</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>#</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -76,6 +72,10 @@
   </si>
   <si>
     <t>${hello}${home|link}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>XlsxTemplate 测试</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -450,65 +450,65 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.875" customWidth="1"/>
-    <col min="2" max="2" width="20.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.875" customWidth="1"/>
+    <col min="1" max="1" width="6.86328125" customWidth="1"/>
+    <col min="2" max="2" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="22.5" x14ac:dyDescent="0.6">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="2">
         <f>ROW()-2</f>
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="2">
         <f>ROW()-2</f>
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="2">
         <f>ROW()-2</f>
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -529,65 +529,65 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.875" customWidth="1"/>
-    <col min="2" max="2" width="20.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.875" customWidth="1"/>
+    <col min="1" max="1" width="6.86328125" customWidth="1"/>
+    <col min="2" max="2" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="22.5" x14ac:dyDescent="0.6">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="2">
         <f>ROW()-2</f>
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="2">
         <f>ROW()-2</f>
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="2">
         <f>ROW()-2</f>
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>